<commit_message>
Added population averaging to supplement-8.
</commit_message>
<xml_diff>
--- a/bin/competing_risks_calculations.xlsx
+++ b/bin/competing_risks_calculations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\survival-models\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF9EE8AE-3CEA-43F0-8ABF-40076E0DE228}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{244B12C3-2AD1-4906-BC00-7C53E5785636}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810"/>
   </bookViews>
@@ -923,7 +923,7 @@
   <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,7 +1094,7 @@
         <v>0.73123287671232884</v>
       </c>
       <c r="H4" s="1" t="str">
-        <f t="shared" ref="H4:H29" si="0">_xlfn.CONCAT(C4, "/",F4,"*",ROUND(G3,3),"=", ROUND(S4, 3))</f>
+        <f>_xlfn.CONCAT(C4, "/",F4,"*",ROUND(G3,3),"=", ROUND(S4, 3))</f>
         <v>15/350*0.815=0.035</v>
       </c>
       <c r="I4" s="1" t="str">
@@ -1102,7 +1102,7 @@
         <v>0.035+0.078=0.113</v>
       </c>
       <c r="J4" s="1" t="str">
-        <f t="shared" ref="J4:J29" si="1">_xlfn.CONCAT(D4, "/",F4,"*",ROUND(G3,3),"=", ROUND(T4, 3))</f>
+        <f>_xlfn.CONCAT(D4, "/",F4,"*",ROUND(G3,3),"=", ROUND(T4, 3))</f>
         <v>1/350*0.815=0.002</v>
       </c>
       <c r="K4" s="1" t="str">
@@ -1110,7 +1110,7 @@
         <v>0.002+0.005=0.007</v>
       </c>
       <c r="L4" s="1" t="str">
-        <f t="shared" ref="L4:L29" si="2">_xlfn.CONCAT(E4, "/",F4,"*",ROUND(G3,3),"=", ROUND(U4, 3))</f>
+        <f>_xlfn.CONCAT(E4, "/",F4,"*",ROUND(G3,3),"=", ROUND(U4, 3))</f>
         <v>20/350*0.815=0.047</v>
       </c>
       <c r="M4" s="1" t="str">
@@ -1166,27 +1166,27 @@
         <v>0.64223413842826249</v>
       </c>
       <c r="H5" s="1" t="str">
-        <f t="shared" si="0"/>
+        <f>_xlfn.CONCAT(C5, "/",F5,"*",ROUND(G4,3),"=", ROUND(S5, 3))</f>
         <v>15/304*0.731=0.036</v>
       </c>
       <c r="I5" s="1" t="str">
-        <f t="shared" ref="I5:I29" si="3">_xlfn.CONCAT(ROUND(S5, 3),"+",ROUND(O4,3),"=",ROUND(O5,3))</f>
+        <f t="shared" ref="I5:I29" si="0">_xlfn.CONCAT(ROUND(S5, 3),"+",ROUND(O4,3),"=",ROUND(O5,3))</f>
         <v>0.036+0.113=0.149</v>
       </c>
       <c r="J5" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(D5, "/",F5,"*",ROUND(G4,3),"=", ROUND(T5, 3))</f>
         <v>2/304*0.731=0.005</v>
       </c>
       <c r="K5" s="1" t="str">
-        <f t="shared" ref="K5:K29" si="4">_xlfn.CONCAT(ROUND(T5, 3),"+",ROUND(P4,3),"=",ROUND(P5,3))</f>
+        <f t="shared" ref="K5:K29" si="1">_xlfn.CONCAT(ROUND(T5, 3),"+",ROUND(P4,3),"=",ROUND(P5,3))</f>
         <v>0.005+0.007=0.012</v>
       </c>
       <c r="L5" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(E5, "/",F5,"*",ROUND(G4,3),"=", ROUND(U5, 3))</f>
         <v>20/304*0.731=0.048</v>
       </c>
       <c r="M5" s="1" t="str">
-        <f t="shared" ref="M5:M29" si="5">_xlfn.CONCAT(ROUND(U5, 3),"+",ROUND(Q4,3),"=",ROUND(Q5,3))</f>
+        <f t="shared" ref="M5:M29" si="2">_xlfn.CONCAT(ROUND(U5, 3),"+",ROUND(Q4,3),"=",ROUND(Q5,3))</f>
         <v>0.048+0.149=0.197</v>
       </c>
       <c r="O5" s="2">
@@ -1238,27 +1238,27 @@
         <v>0.56008791141999636</v>
       </c>
       <c r="H6" s="1" t="str">
+        <f>_xlfn.CONCAT(C6, "/",F6,"*",ROUND(G5,3),"=", ROUND(S6, 3))</f>
+        <v>17/258*0.642=0.042</v>
+      </c>
+      <c r="I6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>17/258*0.642=0.042</v>
-      </c>
-      <c r="I6" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.042+0.149=0.191</v>
       </c>
       <c r="J6" s="1" t="str">
+        <f>_xlfn.CONCAT(D6, "/",F6,"*",ROUND(G5,3),"=", ROUND(T6, 3))</f>
+        <v>4/258*0.642=0.01</v>
+      </c>
+      <c r="K6" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>4/258*0.642=0.01</v>
-      </c>
-      <c r="K6" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.01+0.012=0.022</v>
       </c>
       <c r="L6" s="1" t="str">
+        <f>_xlfn.CONCAT(E6, "/",F6,"*",ROUND(G5,3),"=", ROUND(U6, 3))</f>
+        <v>12/258*0.642=0.03</v>
+      </c>
+      <c r="M6" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>12/258*0.642=0.03</v>
-      </c>
-      <c r="M6" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.03+0.197=0.227</v>
       </c>
       <c r="O6" s="2">
@@ -1310,27 +1310,27 @@
         <v>0.46975115151354535</v>
       </c>
       <c r="H7" s="1" t="str">
+        <f>_xlfn.CONCAT(C7, "/",F7,"*",ROUND(G6,3),"=", ROUND(S7, 3))</f>
+        <v>24/217*0.56=0.062</v>
+      </c>
+      <c r="I7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>24/217*0.56=0.062</v>
-      </c>
-      <c r="I7" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.062+0.191=0.253</v>
       </c>
       <c r="J7" s="1" t="str">
+        <f>_xlfn.CONCAT(D7, "/",F7,"*",ROUND(G6,3),"=", ROUND(T7, 3))</f>
+        <v>2/217*0.56=0.005</v>
+      </c>
+      <c r="K7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2/217*0.56=0.005</v>
-      </c>
-      <c r="K7" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.005+0.022=0.027</v>
       </c>
       <c r="L7" s="1" t="str">
+        <f>_xlfn.CONCAT(E7, "/",F7,"*",ROUND(G6,3),"=", ROUND(U7, 3))</f>
+        <v>9/217*0.56=0.023</v>
+      </c>
+      <c r="M7" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>9/217*0.56=0.023</v>
-      </c>
-      <c r="M7" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.023+0.227=0.251</v>
       </c>
       <c r="O7" s="2">
@@ -1382,27 +1382,27 @@
         <v>0.39278627358194756</v>
       </c>
       <c r="H8" s="1" t="str">
+        <f>_xlfn.CONCAT(C8, "/",F8,"*",ROUND(G7,3),"=", ROUND(S8, 3))</f>
+        <v>17/177*0.47=0.045</v>
+      </c>
+      <c r="I8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>17/177*0.47=0.045</v>
-      </c>
-      <c r="I8" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.045+0.253=0.298</v>
       </c>
       <c r="J8" s="1" t="str">
+        <f>_xlfn.CONCAT(D8, "/",F8,"*",ROUND(G7,3),"=", ROUND(T8, 3))</f>
+        <v>1/177*0.47=0.003</v>
+      </c>
+      <c r="K8" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1/177*0.47=0.003</v>
-      </c>
-      <c r="K8" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.003+0.027=0.029</v>
       </c>
       <c r="L8" s="1" t="str">
+        <f>_xlfn.CONCAT(E8, "/",F8,"*",ROUND(G7,3),"=", ROUND(U8, 3))</f>
+        <v>11/177*0.47=0.029</v>
+      </c>
+      <c r="M8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>11/177*0.47=0.029</v>
-      </c>
-      <c r="M8" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.029+0.251=0.28</v>
       </c>
       <c r="O8" s="2">
@@ -1454,27 +1454,27 @@
         <v>0.3478964137440107</v>
       </c>
       <c r="H9" s="1" t="str">
+        <f>_xlfn.CONCAT(C9, "/",F9,"*",ROUND(G8,3),"=", ROUND(S9, 3))</f>
+        <v>8/140*0.393=0.022</v>
+      </c>
+      <c r="I9" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>8/140*0.393=0.022</v>
-      </c>
-      <c r="I9" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.022+0.298=0.32</v>
       </c>
       <c r="J9" s="1" t="str">
+        <f>_xlfn.CONCAT(D9, "/",F9,"*",ROUND(G8,3),"=", ROUND(T9, 3))</f>
+        <v>2/140*0.393=0.006</v>
+      </c>
+      <c r="K9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2/140*0.393=0.006</v>
-      </c>
-      <c r="K9" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.006+0.029=0.035</v>
       </c>
       <c r="L9" s="1" t="str">
+        <f>_xlfn.CONCAT(E9, "/",F9,"*",ROUND(G8,3),"=", ROUND(U9, 3))</f>
+        <v>6/140*0.393=0.017</v>
+      </c>
+      <c r="M9" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6/140*0.393=0.017</v>
-      </c>
-      <c r="M9" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.017+0.28=0.297</v>
       </c>
       <c r="O9" s="2">
@@ -1526,27 +1526,27 @@
         <v>0.33005557201354863</v>
       </c>
       <c r="H10" s="1" t="str">
+        <f>_xlfn.CONCAT(C10, "/",F10,"*",ROUND(G9,3),"=", ROUND(S10, 3))</f>
+        <v>0/117*0.348=0</v>
+      </c>
+      <c r="I10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0/117*0.348=0</v>
-      </c>
-      <c r="I10" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0+0.32=0.32</v>
       </c>
       <c r="J10" s="1" t="str">
+        <f>_xlfn.CONCAT(D10, "/",F10,"*",ROUND(G9,3),"=", ROUND(T10, 3))</f>
+        <v>2/117*0.348=0.006</v>
+      </c>
+      <c r="K10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2/117*0.348=0.006</v>
-      </c>
-      <c r="K10" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.006+0.035=0.041</v>
       </c>
       <c r="L10" s="1" t="str">
+        <f>_xlfn.CONCAT(E10, "/",F10,"*",ROUND(G9,3),"=", ROUND(U10, 3))</f>
+        <v>4/117*0.348=0.012</v>
+      </c>
+      <c r="M10" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4/117*0.348=0.012</v>
-      </c>
-      <c r="M10" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.012+0.297=0.308</v>
       </c>
       <c r="O10" s="2">
@@ -1598,27 +1598,27 @@
         <v>0.30149307058929919</v>
       </c>
       <c r="H11" s="1" t="str">
+        <f>_xlfn.CONCAT(C11, "/",F11,"*",ROUND(G10,3),"=", ROUND(S11, 3))</f>
+        <v>4/104*0.33=0.013</v>
+      </c>
+      <c r="I11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>4/104*0.33=0.013</v>
-      </c>
-      <c r="I11" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.013+0.32=0.333</v>
       </c>
       <c r="J11" s="1" t="str">
+        <f>_xlfn.CONCAT(D11, "/",F11,"*",ROUND(G10,3),"=", ROUND(T11, 3))</f>
+        <v>0/104*0.33=0</v>
+      </c>
+      <c r="K11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>0/104*0.33=0</v>
-      </c>
-      <c r="K11" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0+0.041=0.041</v>
       </c>
       <c r="L11" s="1" t="str">
+        <f>_xlfn.CONCAT(E11, "/",F11,"*",ROUND(G10,3),"=", ROUND(U11, 3))</f>
+        <v>5/104*0.33=0.016</v>
+      </c>
+      <c r="M11" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>5/104*0.33=0.016</v>
-      </c>
-      <c r="M11" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.016+0.308=0.324</v>
       </c>
       <c r="O11" s="2">
@@ -1670,27 +1670,27 @@
         <v>0.29109675781035788</v>
       </c>
       <c r="H12" s="1" t="str">
+        <f>_xlfn.CONCAT(C12, "/",F12,"*",ROUND(G11,3),"=", ROUND(S12, 3))</f>
+        <v>0/87*0.301=0</v>
+      </c>
+      <c r="I12" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0/87*0.301=0</v>
-      </c>
-      <c r="I12" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0+0.333=0.333</v>
       </c>
       <c r="J12" s="1" t="str">
+        <f>_xlfn.CONCAT(D12, "/",F12,"*",ROUND(G11,3),"=", ROUND(T12, 3))</f>
+        <v>1/87*0.301=0.003</v>
+      </c>
+      <c r="K12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1/87*0.301=0.003</v>
-      </c>
-      <c r="K12" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.003+0.041=0.045</v>
       </c>
       <c r="L12" s="1" t="str">
+        <f>_xlfn.CONCAT(E12, "/",F12,"*",ROUND(G11,3),"=", ROUND(U12, 3))</f>
+        <v>2/87*0.301=0.007</v>
+      </c>
+      <c r="M12" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2/87*0.301=0.007</v>
-      </c>
-      <c r="M12" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.007+0.324=0.331</v>
       </c>
       <c r="O12" s="2">
@@ -1742,27 +1742,27 @@
         <v>0.26870469951725345</v>
       </c>
       <c r="H13" s="1" t="str">
+        <f>_xlfn.CONCAT(C13, "/",F13,"*",ROUND(G12,3),"=", ROUND(S13, 3))</f>
+        <v>2/78*0.291=0.007</v>
+      </c>
+      <c r="I13" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2/78*0.291=0.007</v>
-      </c>
-      <c r="I13" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.007+0.333=0.341</v>
       </c>
       <c r="J13" s="1" t="str">
+        <f>_xlfn.CONCAT(D13, "/",F13,"*",ROUND(G12,3),"=", ROUND(T13, 3))</f>
+        <v>0/78*0.291=0</v>
+      </c>
+      <c r="K13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>0/78*0.291=0</v>
-      </c>
-      <c r="K13" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0+0.045=0.045</v>
       </c>
       <c r="L13" s="1" t="str">
+        <f>_xlfn.CONCAT(E13, "/",F13,"*",ROUND(G12,3),"=", ROUND(U13, 3))</f>
+        <v>4/78*0.291=0.015</v>
+      </c>
+      <c r="M13" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>4/78*0.291=0.015</v>
-      </c>
-      <c r="M13" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.015+0.331=0.346</v>
       </c>
       <c r="O13" s="2">
@@ -1814,27 +1814,27 @@
         <v>0.23261003838807018</v>
       </c>
       <c r="H14" s="1" t="str">
+        <f>_xlfn.CONCAT(C14, "/",F14,"*",ROUND(G13,3),"=", ROUND(S14, 3))</f>
+        <v>2/67*0.269=0.008</v>
+      </c>
+      <c r="I14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2/67*0.269=0.008</v>
-      </c>
-      <c r="I14" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.008+0.341=0.349</v>
       </c>
       <c r="J14" s="1" t="str">
+        <f>_xlfn.CONCAT(D14, "/",F14,"*",ROUND(G13,3),"=", ROUND(T14, 3))</f>
+        <v>1/67*0.269=0.004</v>
+      </c>
+      <c r="K14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1/67*0.269=0.004</v>
-      </c>
-      <c r="K14" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.004+0.045=0.049</v>
       </c>
       <c r="L14" s="1" t="str">
+        <f>_xlfn.CONCAT(E14, "/",F14,"*",ROUND(G13,3),"=", ROUND(U14, 3))</f>
+        <v>6/67*0.269=0.024</v>
+      </c>
+      <c r="M14" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>6/67*0.269=0.024</v>
-      </c>
-      <c r="M14" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.024+0.346=0.37</v>
       </c>
       <c r="O14" s="2">
@@ -1886,27 +1886,27 @@
         <v>0.21656796677509982</v>
       </c>
       <c r="H15" s="1" t="str">
+        <f>_xlfn.CONCAT(C15, "/",F15,"*",ROUND(G14,3),"=", ROUND(S15, 3))</f>
+        <v>1/58*0.233=0.004</v>
+      </c>
+      <c r="I15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1/58*0.233=0.004</v>
-      </c>
-      <c r="I15" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.004+0.349=0.353</v>
       </c>
       <c r="J15" s="1" t="str">
+        <f>_xlfn.CONCAT(D15, "/",F15,"*",ROUND(G14,3),"=", ROUND(T15, 3))</f>
+        <v>3/58*0.233=0.012</v>
+      </c>
+      <c r="K15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3/58*0.233=0.012</v>
-      </c>
-      <c r="K15" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.012+0.049=0.061</v>
       </c>
       <c r="L15" s="1" t="str">
+        <f>_xlfn.CONCAT(E15, "/",F15,"*",ROUND(G14,3),"=", ROUND(U15, 3))</f>
+        <v>0/58*0.233=0</v>
+      </c>
+      <c r="M15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/58*0.233=0</v>
-      </c>
-      <c r="M15" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.37=0.37</v>
       </c>
       <c r="O15" s="2">
@@ -1958,27 +1958,27 @@
         <v>0.19888894907917332</v>
       </c>
       <c r="H16" s="1" t="str">
+        <f>_xlfn.CONCAT(C16, "/",F16,"*",ROUND(G15,3),"=", ROUND(S16, 3))</f>
+        <v>0/49*0.217=0</v>
+      </c>
+      <c r="I16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0/49*0.217=0</v>
-      </c>
-      <c r="I16" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0+0.353=0.353</v>
       </c>
       <c r="J16" s="1" t="str">
+        <f>_xlfn.CONCAT(D16, "/",F16,"*",ROUND(G15,3),"=", ROUND(T16, 3))</f>
+        <v>1/49*0.217=0.004</v>
+      </c>
+      <c r="K16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>1/49*0.217=0.004</v>
-      </c>
-      <c r="K16" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0.004+0.061=0.065</v>
       </c>
       <c r="L16" s="1" t="str">
+        <f>_xlfn.CONCAT(E16, "/",F16,"*",ROUND(G15,3),"=", ROUND(U16, 3))</f>
+        <v>3/49*0.217=0.013</v>
+      </c>
+      <c r="M16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>3/49*0.217=0.013</v>
-      </c>
-      <c r="M16" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.013+0.37=0.383</v>
       </c>
       <c r="O16" s="2">
@@ -2030,27 +2030,27 @@
         <v>0.1808081355265212</v>
       </c>
       <c r="H17" s="1" t="str">
+        <f>_xlfn.CONCAT(C17, "/",F17,"*",ROUND(G16,3),"=", ROUND(S17, 3))</f>
+        <v>1/44*0.199=0.005</v>
+      </c>
+      <c r="I17" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0.005+0.353=0.357</v>
+      </c>
+      <c r="J17" s="1" t="str">
+        <f>_xlfn.CONCAT(D17, "/",F17,"*",ROUND(G16,3),"=", ROUND(T17, 3))</f>
+        <v>2/44*0.199=0.009</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>0.009+0.065=0.074</v>
+      </c>
+      <c r="L17" s="1" t="str">
+        <f>_xlfn.CONCAT(E17, "/",F17,"*",ROUND(G16,3),"=", ROUND(U17, 3))</f>
         <v>1/44*0.199=0.005</v>
       </c>
-      <c r="I17" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0.005+0.353=0.357</v>
-      </c>
-      <c r="J17" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>2/44*0.199=0.009</v>
-      </c>
-      <c r="K17" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0.009+0.065=0.074</v>
-      </c>
-      <c r="L17" s="1" t="str">
+      <c r="M17" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1/44*0.199=0.005</v>
-      </c>
-      <c r="M17" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.005+0.383=0.388</v>
       </c>
       <c r="O17" s="2">
@@ -2102,27 +2102,27 @@
         <v>0.17129191786723061</v>
       </c>
       <c r="H18" s="1" t="str">
+        <f>_xlfn.CONCAT(C18, "/",F18,"*",ROUND(G17,3),"=", ROUND(S18, 3))</f>
+        <v>0/38*0.181=0</v>
+      </c>
+      <c r="I18" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0+0.357=0.357</v>
+      </c>
+      <c r="J18" s="1" t="str">
+        <f>_xlfn.CONCAT(D18, "/",F18,"*",ROUND(G17,3),"=", ROUND(T18, 3))</f>
         <v>0/38*0.181=0</v>
       </c>
-      <c r="I18" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0+0.357=0.357</v>
-      </c>
-      <c r="J18" s="1" t="str">
+      <c r="K18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>0/38*0.181=0</v>
-      </c>
-      <c r="K18" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0+0.074=0.074</v>
       </c>
       <c r="L18" s="1" t="str">
+        <f>_xlfn.CONCAT(E18, "/",F18,"*",ROUND(G17,3),"=", ROUND(U18, 3))</f>
+        <v>2/38*0.181=0.01</v>
+      </c>
+      <c r="M18" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2/38*0.181=0.01</v>
-      </c>
-      <c r="M18" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.01+0.388=0.398</v>
       </c>
       <c r="O18" s="2">
@@ -2174,27 +2174,27 @@
         <v>0.16593904543387966</v>
       </c>
       <c r="H19" s="1" t="str">
+        <f>_xlfn.CONCAT(C19, "/",F19,"*",ROUND(G18,3),"=", ROUND(S19, 3))</f>
+        <v>0/32*0.171=0</v>
+      </c>
+      <c r="I19" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0+0.357=0.357</v>
+      </c>
+      <c r="J19" s="1" t="str">
+        <f>_xlfn.CONCAT(D19, "/",F19,"*",ROUND(G18,3),"=", ROUND(T19, 3))</f>
         <v>0/32*0.171=0</v>
       </c>
-      <c r="I19" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0+0.357=0.357</v>
-      </c>
-      <c r="J19" s="1" t="str">
+      <c r="K19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>0/32*0.171=0</v>
-      </c>
-      <c r="K19" s="1" t="str">
-        <f t="shared" si="4"/>
         <v>0+0.074=0.074</v>
       </c>
       <c r="L19" s="1" t="str">
+        <f>_xlfn.CONCAT(E19, "/",F19,"*",ROUND(G18,3),"=", ROUND(U19, 3))</f>
+        <v>1/32*0.171=0.005</v>
+      </c>
+      <c r="M19" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1/32*0.171=0.005</v>
-      </c>
-      <c r="M19" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.005+0.398=0.403</v>
       </c>
       <c r="O19" s="2">
@@ -2246,27 +2246,27 @@
         <v>0.14305090123610315</v>
       </c>
       <c r="H20" s="1" t="str">
+        <f>_xlfn.CONCAT(C20, "/",F20,"*",ROUND(G19,3),"=", ROUND(S20, 3))</f>
+        <v>2/29*0.166=0.011</v>
+      </c>
+      <c r="I20" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2/29*0.166=0.011</v>
-      </c>
-      <c r="I20" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.011+0.357=0.369</v>
       </c>
       <c r="J20" s="1" t="str">
+        <f>_xlfn.CONCAT(D20, "/",F20,"*",ROUND(G19,3),"=", ROUND(T20, 3))</f>
+        <v>1/29*0.166=0.006</v>
+      </c>
+      <c r="K20" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0.006+0.074=0.08</v>
+      </c>
+      <c r="L20" s="1" t="str">
+        <f>_xlfn.CONCAT(E20, "/",F20,"*",ROUND(G19,3),"=", ROUND(U20, 3))</f>
         <v>1/29*0.166=0.006</v>
       </c>
-      <c r="K20" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0.006+0.074=0.08</v>
-      </c>
-      <c r="L20" s="1" t="str">
+      <c r="M20" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1/29*0.166=0.006</v>
-      </c>
-      <c r="M20" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.006+0.403=0.409</v>
       </c>
       <c r="O20" s="2">
@@ -2318,27 +2318,27 @@
         <v>0.13061169243296375</v>
       </c>
       <c r="H21" s="1" t="str">
+        <f>_xlfn.CONCAT(C21, "/",F21,"*",ROUND(G20,3),"=", ROUND(S21, 3))</f>
+        <v>0/23*0.143=0</v>
+      </c>
+      <c r="I21" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0/23*0.143=0</v>
-      </c>
-      <c r="I21" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0+0.369=0.369</v>
       </c>
       <c r="J21" s="1" t="str">
+        <f>_xlfn.CONCAT(D21, "/",F21,"*",ROUND(G20,3),"=", ROUND(T21, 3))</f>
+        <v>1/23*0.143=0.006</v>
+      </c>
+      <c r="K21" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0.006+0.08=0.086</v>
+      </c>
+      <c r="L21" s="1" t="str">
+        <f>_xlfn.CONCAT(E21, "/",F21,"*",ROUND(G20,3),"=", ROUND(U21, 3))</f>
         <v>1/23*0.143=0.006</v>
       </c>
-      <c r="K21" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0.006+0.08=0.086</v>
-      </c>
-      <c r="L21" s="1" t="str">
+      <c r="M21" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1/23*0.143=0.006</v>
-      </c>
-      <c r="M21" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.006+0.409=0.415</v>
       </c>
       <c r="O21" s="2">
@@ -2390,27 +2390,27 @@
         <v>0.11686309322949388</v>
       </c>
       <c r="H22" s="1" t="str">
+        <f>_xlfn.CONCAT(C22, "/",F22,"*",ROUND(G21,3),"=", ROUND(S22, 3))</f>
+        <v>0/19*0.131=0</v>
+      </c>
+      <c r="I22" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>0/19*0.131=0</v>
-      </c>
-      <c r="I22" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0+0.369=0.369</v>
       </c>
       <c r="J22" s="1" t="str">
+        <f>_xlfn.CONCAT(D22, "/",F22,"*",ROUND(G21,3),"=", ROUND(T22, 3))</f>
+        <v>1/19*0.131=0.007</v>
+      </c>
+      <c r="K22" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0.007+0.086=0.093</v>
+      </c>
+      <c r="L22" s="1" t="str">
+        <f>_xlfn.CONCAT(E22, "/",F22,"*",ROUND(G21,3),"=", ROUND(U22, 3))</f>
         <v>1/19*0.131=0.007</v>
       </c>
-      <c r="K22" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0.007+0.086=0.093</v>
-      </c>
-      <c r="L22" s="1" t="str">
+      <c r="M22" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>1/19*0.131=0.007</v>
-      </c>
-      <c r="M22" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0.007+0.415=0.422</v>
       </c>
       <c r="O22" s="2">
@@ -2462,27 +2462,27 @@
         <v>0.10128134746556137</v>
       </c>
       <c r="H23" s="1" t="str">
+        <f>_xlfn.CONCAT(C23, "/",F23,"*",ROUND(G22,3),"=", ROUND(S23, 3))</f>
+        <v>2/15*0.117=0.016</v>
+      </c>
+      <c r="I23" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>2/15*0.117=0.016</v>
-      </c>
-      <c r="I23" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.016+0.369=0.384</v>
       </c>
       <c r="J23" s="1" t="str">
+        <f>_xlfn.CONCAT(D23, "/",F23,"*",ROUND(G22,3),"=", ROUND(T23, 3))</f>
+        <v>0/15*0.117=0</v>
+      </c>
+      <c r="K23" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L23" s="1" t="str">
+        <f>_xlfn.CONCAT(E23, "/",F23,"*",ROUND(G22,3),"=", ROUND(U23, 3))</f>
         <v>0/15*0.117=0</v>
       </c>
-      <c r="K23" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L23" s="1" t="str">
+      <c r="M23" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/15*0.117=0</v>
-      </c>
-      <c r="M23" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O23" s="2">
@@ -2534,27 +2534,27 @@
         <v>0.10128134746556137</v>
       </c>
       <c r="H24" s="1" t="str">
+        <f>_xlfn.CONCAT(C24, "/",F24,"*",ROUND(G23,3),"=", ROUND(S24, 3))</f>
+        <v>0/10*0.101=0</v>
+      </c>
+      <c r="I24" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0+0.384=0.384</v>
+      </c>
+      <c r="J24" s="1" t="str">
+        <f>_xlfn.CONCAT(D24, "/",F24,"*",ROUND(G23,3),"=", ROUND(T24, 3))</f>
         <v>0/10*0.101=0</v>
       </c>
-      <c r="I24" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0+0.384=0.384</v>
-      </c>
-      <c r="J24" s="1" t="str">
+      <c r="K24" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L24" s="1" t="str">
+        <f>_xlfn.CONCAT(E24, "/",F24,"*",ROUND(G23,3),"=", ROUND(U24, 3))</f>
         <v>0/10*0.101=0</v>
       </c>
-      <c r="K24" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L24" s="1" t="str">
+      <c r="M24" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/10*0.101=0</v>
-      </c>
-      <c r="M24" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O24" s="2">
@@ -2606,27 +2606,27 @@
         <v>9.0027864413832329E-2</v>
       </c>
       <c r="H25" s="1" t="str">
+        <f>_xlfn.CONCAT(C25, "/",F25,"*",ROUND(G24,3),"=", ROUND(S25, 3))</f>
+        <v>1/9*0.101=0.011</v>
+      </c>
+      <c r="I25" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1/9*0.101=0.011</v>
-      </c>
-      <c r="I25" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.011+0.384=0.395</v>
       </c>
       <c r="J25" s="1" t="str">
+        <f>_xlfn.CONCAT(D25, "/",F25,"*",ROUND(G24,3),"=", ROUND(T25, 3))</f>
+        <v>0/9*0.101=0</v>
+      </c>
+      <c r="K25" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L25" s="1" t="str">
+        <f>_xlfn.CONCAT(E25, "/",F25,"*",ROUND(G24,3),"=", ROUND(U25, 3))</f>
         <v>0/9*0.101=0</v>
       </c>
-      <c r="K25" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L25" s="1" t="str">
+      <c r="M25" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/9*0.101=0</v>
-      </c>
-      <c r="M25" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O25" s="2">
@@ -2678,27 +2678,27 @@
         <v>9.0027864413832329E-2</v>
       </c>
       <c r="H26" s="1" t="str">
+        <f>_xlfn.CONCAT(C26, "/",F26,"*",ROUND(G25,3),"=", ROUND(S26, 3))</f>
+        <v>0/6*0.09=0</v>
+      </c>
+      <c r="I26" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0+0.395=0.395</v>
+      </c>
+      <c r="J26" s="1" t="str">
+        <f>_xlfn.CONCAT(D26, "/",F26,"*",ROUND(G25,3),"=", ROUND(T26, 3))</f>
         <v>0/6*0.09=0</v>
       </c>
-      <c r="I26" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0+0.395=0.395</v>
-      </c>
-      <c r="J26" s="1" t="str">
+      <c r="K26" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L26" s="1" t="str">
+        <f>_xlfn.CONCAT(E26, "/",F26,"*",ROUND(G25,3),"=", ROUND(U26, 3))</f>
         <v>0/6*0.09=0</v>
       </c>
-      <c r="K26" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L26" s="1" t="str">
+      <c r="M26" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/6*0.09=0</v>
-      </c>
-      <c r="M26" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O26" s="2">
@@ -2750,27 +2750,27 @@
         <v>6.752089831037425E-2</v>
       </c>
       <c r="H27" s="1" t="str">
+        <f>_xlfn.CONCAT(C27, "/",F27,"*",ROUND(G26,3),"=", ROUND(S27, 3))</f>
+        <v>1/4*0.09=0.023</v>
+      </c>
+      <c r="I27" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>1/4*0.09=0.023</v>
-      </c>
-      <c r="I27" s="1" t="str">
-        <f t="shared" si="3"/>
         <v>0.023+0.395=0.418</v>
       </c>
       <c r="J27" s="1" t="str">
+        <f>_xlfn.CONCAT(D27, "/",F27,"*",ROUND(G26,3),"=", ROUND(T27, 3))</f>
+        <v>0/4*0.09=0</v>
+      </c>
+      <c r="K27" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L27" s="1" t="str">
+        <f>_xlfn.CONCAT(E27, "/",F27,"*",ROUND(G26,3),"=", ROUND(U27, 3))</f>
         <v>0/4*0.09=0</v>
       </c>
-      <c r="K27" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L27" s="1" t="str">
+      <c r="M27" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/4*0.09=0</v>
-      </c>
-      <c r="M27" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O27" s="2">
@@ -2822,27 +2822,27 @@
         <v>6.752089831037425E-2</v>
       </c>
       <c r="H28" s="1" t="str">
+        <f>_xlfn.CONCAT(C28, "/",F28,"*",ROUND(G27,3),"=", ROUND(S28, 3))</f>
+        <v>0/2*0.068=0</v>
+      </c>
+      <c r="I28" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0+0.418=0.418</v>
+      </c>
+      <c r="J28" s="1" t="str">
+        <f>_xlfn.CONCAT(D28, "/",F28,"*",ROUND(G27,3),"=", ROUND(T28, 3))</f>
         <v>0/2*0.068=0</v>
       </c>
-      <c r="I28" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0+0.418=0.418</v>
-      </c>
-      <c r="J28" s="1" t="str">
+      <c r="K28" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L28" s="1" t="str">
+        <f>_xlfn.CONCAT(E28, "/",F28,"*",ROUND(G27,3),"=", ROUND(U28, 3))</f>
         <v>0/2*0.068=0</v>
       </c>
-      <c r="K28" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L28" s="1" t="str">
+      <c r="M28" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/2*0.068=0</v>
-      </c>
-      <c r="M28" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O28" s="2">
@@ -2894,27 +2894,27 @@
         <v>6.752089831037425E-2</v>
       </c>
       <c r="H29" s="1" t="str">
+        <f>_xlfn.CONCAT(C29, "/",F29,"*",ROUND(G28,3),"=", ROUND(S29, 3))</f>
+        <v>0/1*0.068=0</v>
+      </c>
+      <c r="I29" s="1" t="str">
         <f t="shared" si="0"/>
+        <v>0+0.418=0.418</v>
+      </c>
+      <c r="J29" s="1" t="str">
+        <f>_xlfn.CONCAT(D29, "/",F29,"*",ROUND(G28,3),"=", ROUND(T29, 3))</f>
         <v>0/1*0.068=0</v>
       </c>
-      <c r="I29" s="1" t="str">
-        <f t="shared" si="3"/>
-        <v>0+0.418=0.418</v>
-      </c>
-      <c r="J29" s="1" t="str">
+      <c r="K29" s="1" t="str">
         <f t="shared" si="1"/>
+        <v>0+0.093=0.093</v>
+      </c>
+      <c r="L29" s="1" t="str">
+        <f>_xlfn.CONCAT(E29, "/",F29,"*",ROUND(G28,3),"=", ROUND(U29, 3))</f>
         <v>0/1*0.068=0</v>
       </c>
-      <c r="K29" s="1" t="str">
-        <f t="shared" si="4"/>
-        <v>0+0.093=0.093</v>
-      </c>
-      <c r="L29" s="1" t="str">
+      <c r="M29" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>0/1*0.068=0</v>
-      </c>
-      <c r="M29" s="1" t="str">
-        <f t="shared" si="5"/>
         <v>0+0.422=0.422</v>
       </c>
       <c r="O29" s="2">

</xml_diff>